<commit_message>
mobile number whats-app number add
</commit_message>
<xml_diff>
--- a/client/src/assets/new data.xlsx
+++ b/client/src/assets/new data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
   <si>
     <t xml:space="preserve">EmployeeId</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">Mobile No.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">whatsApp number</t>
   </si>
   <si>
     <t xml:space="preserve">Net Hours</t>
@@ -227,12 +230,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -425,306 +436,330 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="24.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="22.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="23.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="11.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="24.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="7.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="23.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="3" t="n">
         <v>9876543210</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="3" t="n">
+        <v>9876543210</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>8765432109</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>8765432109</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>8765432109</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>7654321098</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>7654321098</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>7654321098</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>21</v>
+      <c r="M4" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="3" t="n">
         <v>6543210987</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="3" t="n">
+        <v>6543210987</v>
+      </c>
+      <c r="H5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="J5" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>21</v>
+      <c r="K5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="1" t="n">
+      <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="3" t="n">
         <v>5432109876</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="3" t="n">
+        <v>5432109876</v>
+      </c>
+      <c r="H6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="J6" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="L6" s="0" t="s">
-        <v>21</v>
+      <c r="K6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="1" t="n">
+      <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="3" t="n">
         <v>4321098765</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="3" t="n">
+        <v>4321098765</v>
+      </c>
+      <c r="H7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="J7" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>21</v>
+      <c r="K7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="1" t="n">
+      <c r="D8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="3" t="n">
         <v>3210987654</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="3" t="n">
+        <v>3210987654</v>
+      </c>
+      <c r="H8" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H8" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="0" t="s">
+      <c r="I8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K8" s="0" t="s">
+      <c r="J8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L8" s="0" t="s">
+      <c r="L8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M8" s="0" t="s">
+      <c r="M8" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>